<commit_message>
change directory and knowledge graph
</commit_message>
<xml_diff>
--- a/paper/paper.xlsx
+++ b/paper/paper.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\machine learning\paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA5C945-A210-4A06-91FF-8D04A02B46E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2A2B17-EAA3-4DA9-9FE9-5255CD7F09EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="word2vec" sheetId="2" r:id="rId1"/>
     <sheet name="LM" sheetId="1" r:id="rId2"/>
     <sheet name="seq2seq" sheetId="3" r:id="rId3"/>
+    <sheet name="CV" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="134">
   <si>
     <t>Tittle</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -537,6 +538,9 @@
   </si>
   <si>
     <t>Our results add to the well-established evidence that unsupervised pre-training of word vectors is an important ingredient in deep learning for NLP.</t>
+  </si>
+  <si>
+    <t>ImageNet Classification with Deep Convolutional Neural Networks</t>
   </si>
 </sst>
 </file>
@@ -869,7 +873,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AB0BF7B-90A0-40ED-A5F2-27CC2A014513}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D1" sqref="A1:XFD1"/>
     </sheetView>
@@ -1205,9 +1209,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1562,4 +1566,63 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9577A6A-62D8-4125-A155-853D5B40F763}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="8.75" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="57.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="47.25" style="1" customWidth="1"/>
+    <col min="7" max="7" width="45.125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="43.375" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="C2" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>